<commit_message>
all components work, added sleep timer to update total score graph
</commit_message>
<xml_diff>
--- a/outputs/total_score_from_upload.xlsx
+++ b/outputs/total_score_from_upload.xlsx
@@ -602,7 +602,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Aditya Birla Group</t>
         </is>
@@ -705,7 +705,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>BMW Foundation Herbert Quandt</t>
         </is>
@@ -808,7 +808,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Buenos Aires Innovation Park (City of Buenos Aires Government)</t>
         </is>
@@ -911,7 +911,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>C L Sandberg &amp; Associates</t>
         </is>
@@ -1014,15 +1014,13 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Capital One</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>141.0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>111</v>
       </c>
       <c r="C6" t="n">
         <v>110</v>
@@ -1119,7 +1117,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Classroom Inc</t>
         </is>
@@ -1222,7 +1220,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Corning Capital</t>
         </is>
@@ -1325,7 +1323,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Covestro LLC</t>
         </is>
@@ -1428,7 +1426,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>DIGITAL CITIZEN FUND</t>
         </is>
@@ -1531,7 +1529,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Danaher</t>
         </is>
@@ -1634,7 +1632,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Draper Richards Kaplan Foundation</t>
         </is>
@@ -1737,7 +1735,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Fannie Mae</t>
         </is>
@@ -1840,7 +1838,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>Gary Community Investments</t>
         </is>
@@ -1943,7 +1941,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Grupo Salinas</t>
         </is>
@@ -2046,7 +2044,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Heart Institute of the Caribbean</t>
         </is>
@@ -2149,7 +2147,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>Henkel</t>
         </is>
@@ -2252,7 +2250,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Henkel (Charles Paul)</t>
         </is>
@@ -2355,7 +2353,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>IMPACT2030</t>
         </is>
@@ -2458,7 +2456,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Innovation Norway</t>
         </is>
@@ -2561,7 +2559,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>KSF Impact</t>
         </is>
@@ -2664,7 +2662,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Kevin Przybocki</t>
         </is>
@@ -2767,7 +2765,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
         <is>
           <t>LLamasoft</t>
         </is>
@@ -2870,7 +2868,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="inlineStr">
         <is>
           <t>MIT (Ken Zolot)</t>
         </is>
@@ -2973,7 +2971,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>MIT Environmental Solutions Initative (John Fernandez)</t>
         </is>
@@ -3076,7 +3074,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
         <is>
           <t>MIT Governance Lab (GOV/LAB)</t>
         </is>
@@ -3179,7 +3177,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>Mannin Research Inc.</t>
         </is>
@@ -3282,7 +3280,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="inlineStr">
         <is>
           <t>Maria Cecilia Souto Vidigal Foundation</t>
         </is>
@@ -3385,7 +3383,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="inlineStr">
         <is>
           <t>Miniwiz</t>
         </is>
@@ -3488,7 +3486,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>New Orleans Health Department</t>
         </is>
@@ -3591,7 +3589,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="inlineStr">
         <is>
           <t>Northrop Grumman Corporation</t>
         </is>
@@ -3694,7 +3692,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="inlineStr">
         <is>
           <t>Putnam Associates</t>
         </is>
@@ -3797,7 +3795,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="inlineStr">
         <is>
           <t>Robert Wood Johnson Foundation</t>
         </is>
@@ -3900,7 +3898,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="inlineStr">
         <is>
           <t>Save the Children</t>
         </is>
@@ -4003,7 +4001,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="inlineStr">
         <is>
           <t>Schmidt Marine Technology Partners</t>
         </is>
@@ -4106,7 +4104,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="inlineStr">
         <is>
           <t>Sitra</t>
         </is>
@@ -4209,7 +4207,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="inlineStr">
         <is>
           <t>Terranova Corporation</t>
         </is>
@@ -4312,7 +4310,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="inlineStr">
         <is>
           <t>The Kroger Co. Zero Hunger Zero Waste Foundation</t>
         </is>
@@ -4415,7 +4413,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="inlineStr">
         <is>
           <t>The Pershing Square Foundation</t>
         </is>
@@ -4518,7 +4516,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="inlineStr">
         <is>
           <t>Uber</t>
         </is>
@@ -4621,7 +4619,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="inlineStr">
         <is>
           <t>Yum! Brands</t>
         </is>

</xml_diff>

<commit_message>
added fresh version of solver_partner_weights.xlsx and commented out generate weights code
</commit_message>
<xml_diff>
--- a/outputs/total_score_from_upload.xlsx
+++ b/outputs/total_score_from_upload.xlsx
@@ -602,7 +602,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Aditya Birla Group</t>
         </is>
@@ -705,7 +705,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>BMW Foundation Herbert Quandt</t>
         </is>
@@ -808,7 +808,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Buenos Aires Innovation Park (City of Buenos Aires Government)</t>
         </is>
@@ -911,7 +911,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>C L Sandberg &amp; Associates</t>
         </is>
@@ -1014,13 +1014,15 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Capital One</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>111</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>112.0</t>
+        </is>
       </c>
       <c r="C6" t="n">
         <v>110</v>
@@ -1117,7 +1119,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Classroom Inc</t>
         </is>
@@ -1220,7 +1222,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Corning Capital</t>
         </is>
@@ -1323,7 +1325,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Covestro LLC</t>
         </is>
@@ -1426,7 +1428,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>DIGITAL CITIZEN FUND</t>
         </is>
@@ -1529,7 +1531,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Danaher</t>
         </is>
@@ -1632,7 +1634,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Draper Richards Kaplan Foundation</t>
         </is>
@@ -1735,7 +1737,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Fannie Mae</t>
         </is>
@@ -1838,7 +1840,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Gary Community Investments</t>
         </is>
@@ -1941,7 +1943,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Grupo Salinas</t>
         </is>
@@ -2044,7 +2046,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Heart Institute of the Caribbean</t>
         </is>
@@ -2147,7 +2149,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Henkel</t>
         </is>
@@ -2250,7 +2252,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Henkel (Charles Paul)</t>
         </is>
@@ -2353,7 +2355,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>IMPACT2030</t>
         </is>
@@ -2456,7 +2458,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Innovation Norway</t>
         </is>
@@ -2559,7 +2561,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>KSF Impact</t>
         </is>
@@ -2662,7 +2664,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Kevin Przybocki</t>
         </is>
@@ -2765,7 +2767,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>LLamasoft</t>
         </is>
@@ -2868,7 +2870,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>MIT (Ken Zolot)</t>
         </is>
@@ -2971,7 +2973,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>MIT Environmental Solutions Initative (John Fernandez)</t>
         </is>
@@ -3074,7 +3076,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>MIT Governance Lab (GOV/LAB)</t>
         </is>
@@ -3177,7 +3179,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Mannin Research Inc.</t>
         </is>
@@ -3280,7 +3282,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Maria Cecilia Souto Vidigal Foundation</t>
         </is>
@@ -3383,7 +3385,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Miniwiz</t>
         </is>
@@ -3486,7 +3488,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>New Orleans Health Department</t>
         </is>
@@ -3589,7 +3591,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Northrop Grumman Corporation</t>
         </is>
@@ -3692,7 +3694,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Putnam Associates</t>
         </is>
@@ -3795,7 +3797,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Robert Wood Johnson Foundation</t>
         </is>
@@ -3898,7 +3900,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Save the Children</t>
         </is>
@@ -4001,7 +4003,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Schmidt Marine Technology Partners</t>
         </is>
@@ -4104,7 +4106,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Sitra</t>
         </is>
@@ -4207,7 +4209,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Terranova Corporation</t>
         </is>
@@ -4310,7 +4312,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
+      <c r="A38" t="inlineStr">
         <is>
           <t>The Kroger Co. Zero Hunger Zero Waste Foundation</t>
         </is>
@@ -4413,7 +4415,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
+      <c r="A39" t="inlineStr">
         <is>
           <t>The Pershing Square Foundation</t>
         </is>
@@ -4516,7 +4518,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Uber</t>
         </is>
@@ -4619,7 +4621,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
+      <c r="A41" t="inlineStr">
         <is>
           <t>Yum! Brands</t>
         </is>

</xml_diff>

<commit_message>
reverting back to gunicorn
</commit_message>
<xml_diff>
--- a/outputs/total_score_from_upload.xlsx
+++ b/outputs/total_score_from_upload.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+  <si>
+    <t>Org_y</t>
+  </si>
   <si>
     <t>AIR-INK: Air-Pollution to ink</t>
   </si>
@@ -112,9 +115,6 @@
     <t>change:WATER Labs' iThrone: a waste-shrinking toilet</t>
   </si>
   <si>
-    <t>Org_y</t>
-  </si>
-  <si>
     <t>Aditya Birla Group</t>
   </si>
   <si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Yum! Brands</t>
+  </si>
+  <si>
+    <t>412.0</t>
   </si>
 </sst>
 </file>
@@ -598,107 +601,107 @@
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:33">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2">
@@ -799,7 +802,7 @@
       </c>
     </row>
     <row r="3" spans="1:33">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3">
@@ -900,7 +903,7 @@
       </c>
     </row>
     <row r="4" spans="1:33">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4">
@@ -1001,7 +1004,7 @@
       </c>
     </row>
     <row r="5" spans="1:33">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5">
@@ -1102,11 +1105,11 @@
       </c>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6">
-        <v>412</v>
+      <c r="B6" t="s">
+        <v>73</v>
       </c>
       <c r="C6">
         <v>110</v>
@@ -1203,7 +1206,7 @@
       </c>
     </row>
     <row r="7" spans="1:33">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
       <c r="B7">
@@ -1304,7 +1307,7 @@
       </c>
     </row>
     <row r="8" spans="1:33">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
       <c r="B8">
@@ -1405,7 +1408,7 @@
       </c>
     </row>
     <row r="9" spans="1:33">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
       <c r="B9">
@@ -1506,7 +1509,7 @@
       </c>
     </row>
     <row r="10" spans="1:33">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
       <c r="B10">
@@ -1607,7 +1610,7 @@
       </c>
     </row>
     <row r="11" spans="1:33">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
       <c r="B11">
@@ -1708,7 +1711,7 @@
       </c>
     </row>
     <row r="12" spans="1:33">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12">
@@ -1809,7 +1812,7 @@
       </c>
     </row>
     <row r="13" spans="1:33">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
       <c r="B13">
@@ -1910,7 +1913,7 @@
       </c>
     </row>
     <row r="14" spans="1:33">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
       <c r="B14">
@@ -2011,7 +2014,7 @@
       </c>
     </row>
     <row r="15" spans="1:33">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15">
@@ -2112,7 +2115,7 @@
       </c>
     </row>
     <row r="16" spans="1:33">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>47</v>
       </c>
       <c r="B16">
@@ -2213,7 +2216,7 @@
       </c>
     </row>
     <row r="17" spans="1:33">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>48</v>
       </c>
       <c r="B17">
@@ -2314,7 +2317,7 @@
       </c>
     </row>
     <row r="18" spans="1:33">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="B18">
@@ -2415,7 +2418,7 @@
       </c>
     </row>
     <row r="19" spans="1:33">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>50</v>
       </c>
       <c r="B19">
@@ -2516,7 +2519,7 @@
       </c>
     </row>
     <row r="20" spans="1:33">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>51</v>
       </c>
       <c r="B20">
@@ -2617,7 +2620,7 @@
       </c>
     </row>
     <row r="21" spans="1:33">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>52</v>
       </c>
       <c r="B21">
@@ -2718,7 +2721,7 @@
       </c>
     </row>
     <row r="22" spans="1:33">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
       <c r="B22">
@@ -2819,7 +2822,7 @@
       </c>
     </row>
     <row r="23" spans="1:33">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>54</v>
       </c>
       <c r="B23">
@@ -2920,7 +2923,7 @@
       </c>
     </row>
     <row r="24" spans="1:33">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>55</v>
       </c>
       <c r="B24">
@@ -3021,7 +3024,7 @@
       </c>
     </row>
     <row r="25" spans="1:33">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
       <c r="B25">
@@ -3122,7 +3125,7 @@
       </c>
     </row>
     <row r="26" spans="1:33">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
       <c r="B26">
@@ -3223,7 +3226,7 @@
       </c>
     </row>
     <row r="27" spans="1:33">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
       <c r="B27">
@@ -3324,7 +3327,7 @@
       </c>
     </row>
     <row r="28" spans="1:33">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
       <c r="B28">
@@ -3425,7 +3428,7 @@
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>60</v>
       </c>
       <c r="B29">
@@ -3526,7 +3529,7 @@
       </c>
     </row>
     <row r="30" spans="1:33">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>61</v>
       </c>
       <c r="B30">
@@ -3627,7 +3630,7 @@
       </c>
     </row>
     <row r="31" spans="1:33">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>62</v>
       </c>
       <c r="B31">
@@ -3728,7 +3731,7 @@
       </c>
     </row>
     <row r="32" spans="1:33">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>63</v>
       </c>
       <c r="B32">
@@ -3829,7 +3832,7 @@
       </c>
     </row>
     <row r="33" spans="1:33">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>64</v>
       </c>
       <c r="B33">
@@ -3930,7 +3933,7 @@
       </c>
     </row>
     <row r="34" spans="1:33">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
       <c r="B34">
@@ -4031,7 +4034,7 @@
       </c>
     </row>
     <row r="35" spans="1:33">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>66</v>
       </c>
       <c r="B35">
@@ -4132,7 +4135,7 @@
       </c>
     </row>
     <row r="36" spans="1:33">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>67</v>
       </c>
       <c r="B36">
@@ -4233,7 +4236,7 @@
       </c>
     </row>
     <row r="37" spans="1:33">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>68</v>
       </c>
       <c r="B37">
@@ -4334,7 +4337,7 @@
       </c>
     </row>
     <row r="38" spans="1:33">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>69</v>
       </c>
       <c r="B38">
@@ -4435,7 +4438,7 @@
       </c>
     </row>
     <row r="39" spans="1:33">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>70</v>
       </c>
       <c r="B39">
@@ -4536,7 +4539,7 @@
       </c>
     </row>
     <row r="40" spans="1:33">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>71</v>
       </c>
       <c r="B40">
@@ -4637,7 +4640,7 @@
       </c>
     </row>
     <row r="41" spans="1:33">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
       <c r="B41">

</xml_diff>